<commit_message>
combine with Backup_Selection and HW/OS/Client
</commit_message>
<xml_diff>
--- a/testArea/policies.txt.xlsx
+++ b/testArea/policies.txt.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="38">
   <si>
     <t>Policy Name</t>
   </si>
@@ -31,88 +31,103 @@
     <t>Use Accelerator</t>
   </si>
   <si>
-    <t>HW/OS/Client</t>
-  </si>
-  <si>
-    <t>Include</t>
+    <t>HW</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>Client</t>
+  </si>
+  <si>
+    <t>Backup_Selection</t>
   </si>
   <si>
     <t>Schedule</t>
   </si>
   <si>
-    <t xml:space="preserve">       CATALOG_BACKUP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">       HYDRA1_FS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">       HYDRA1_FS_TEST</t>
-  </si>
-  <si>
-    <t xml:space="preserve">       HYDRAMYSQL_MYSQL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">       TEST_LTO4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">       VM-WIN105_SQL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">       catalog2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">       emptySERVER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">       test</t>
-  </si>
-  <si>
-    <t xml:space="preserve">         NBU-Catalog</t>
-  </si>
-  <si>
-    <t xml:space="preserve">         Standard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">         DataStore</t>
-  </si>
-  <si>
-    <t xml:space="preserve">         MS-SQL-Server</t>
-  </si>
-  <si>
-    <t xml:space="preserve">           (specific storage unit not required)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">           HYDRA1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">           LTO4 LTO5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">           MASTER_DISK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">         (same as policy volume pool)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">         NetBackup</t>
-  </si>
-  <si>
-    <t xml:space="preserve">         NetBackup NetBackup</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  no</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Linux         Linux         hydra1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Linux         RedHat2.6.32  hydra1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Linux         RedHat2.6.32  hydramysql</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Linux         RedHat2.6.32  emptyServer</t>
+    <t>CATALOG_BACKUP</t>
+  </si>
+  <si>
+    <t>HYDRA1_FS</t>
+  </si>
+  <si>
+    <t>HYDRA1_FS_TEST</t>
+  </si>
+  <si>
+    <t>HYDRAMYSQL_MYSQL</t>
+  </si>
+  <si>
+    <t>TEST_LTO4</t>
+  </si>
+  <si>
+    <t>VM-WIN105_SQL</t>
+  </si>
+  <si>
+    <t>catalog2</t>
+  </si>
+  <si>
+    <t>emptySERVER</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>NBU-Catalog</t>
+  </si>
+  <si>
+    <t>Standard</t>
+  </si>
+  <si>
+    <t>DataStore</t>
+  </si>
+  <si>
+    <t>MS-SQL-Server</t>
+  </si>
+  <si>
+    <t>LTO5</t>
+  </si>
+  <si>
+    <t>MASTER_DISK</t>
+  </si>
+  <si>
+    <t>HYDRA1</t>
+  </si>
+  <si>
+    <t>LTO4</t>
+  </si>
+  <si>
+    <t>STGUNIT</t>
+  </si>
+  <si>
+    <t>CatalogBackup</t>
+  </si>
+  <si>
+    <t>NetBackup</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>Linux</t>
+  </si>
+  <si>
+    <t>RedHat2.6.32</t>
+  </si>
+  <si>
+    <t>hydra1</t>
+  </si>
+  <si>
+    <t>hydramysql</t>
+  </si>
+  <si>
+    <t>emptyServer</t>
+  </si>
+  <si>
+    <t>(none defined)</t>
+  </si>
+  <si>
+    <t>WHOLE_DATABASE</t>
   </si>
 </sst>
 </file>
@@ -470,237 +485,264 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="1">
-        <v>0</v>
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" t="s">
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" t="s">
+        <v>30</v>
+      </c>
+      <c r="I7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" t="s">
         <v>17</v>
       </c>
-      <c r="D2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" t="s">
-        <v>28</v>
-      </c>
-      <c r="G5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F6" t="s">
-        <v>28</v>
-      </c>
-      <c r="G6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="1">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" t="s">
-        <v>26</v>
-      </c>
-      <c r="F7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="1">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" t="s">
-        <v>25</v>
-      </c>
-      <c r="F8" t="s">
-        <v>28</v>
-      </c>
-      <c r="G8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="1">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" t="s">
-        <v>21</v>
-      </c>
       <c r="E9" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="F9" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="G9" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="1">
-        <v>8</v>
+      <c r="H9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" t="s">
+        <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="D10" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="E10" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="F10" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="G10" t="s">
-        <v>30</v>
+        <v>32</v>
+      </c>
+      <c r="H10" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>